<commit_message>
add tradicional agent and README
</commit_message>
<xml_diff>
--- a/simulacion_AAPL.xlsx
+++ b/simulacion_AAPL.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,492 +461,478 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45847.5625</v>
+        <v>45847.60416666666</v>
       </c>
       <c r="B2" t="n">
+        <v>207.8049926757812</v>
+      </c>
+      <c r="C2" t="n">
         <v>209.9100036621094</v>
       </c>
-      <c r="C2" t="n">
-        <v>214.2739479633478</v>
-      </c>
       <c r="D2" t="n">
-        <v>203.92037052206</v>
+        <v>207.0885515158442</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45847.60416666666</v>
+        <v>45847.64583333334</v>
       </c>
       <c r="B3" t="n">
+        <v>207.8000030517578</v>
+      </c>
+      <c r="C3" t="n">
         <v>207.8049926757812</v>
       </c>
-      <c r="C3" t="n">
-        <v>212.0450203648158</v>
-      </c>
       <c r="D3" t="n">
-        <v>208.8854967211167</v>
+        <v>207.3134535566308</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45847.64583333334</v>
+        <v>45847.6875</v>
       </c>
       <c r="B4" t="n">
+        <v>208.9156036376953</v>
+      </c>
+      <c r="C4" t="n">
         <v>207.8000030517578</v>
       </c>
-      <c r="C4" t="n">
-        <v>203.7514937904261</v>
-      </c>
       <c r="D4" t="n">
-        <v>199.8951983998498</v>
+        <v>198.0988443588153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45847.6875</v>
+        <v>45847.72916666666</v>
       </c>
       <c r="B5" t="n">
+        <v>209.7324981689453</v>
+      </c>
+      <c r="C5" t="n">
         <v>208.9156036376953</v>
       </c>
-      <c r="C5" t="n">
-        <v>207.6249974406629</v>
-      </c>
       <c r="D5" t="n">
-        <v>202.1655288729558</v>
+        <v>213.1562751313305</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45847.72916666666</v>
+        <v>45847.77083333334</v>
       </c>
       <c r="B6" t="n">
+        <v>209.8899993896484</v>
+      </c>
+      <c r="C6" t="n">
         <v>209.7324981689453</v>
       </c>
-      <c r="C6" t="n">
-        <v>208.3953284045456</v>
-      </c>
       <c r="D6" t="n">
-        <v>209.401692148475</v>
+        <v>209.9908352218939</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45847.77083333334</v>
+        <v>45847.8125</v>
       </c>
       <c r="B7" t="n">
+        <v>211.1100006103516</v>
+      </c>
+      <c r="C7" t="n">
         <v>209.8899993896484</v>
       </c>
-      <c r="C7" t="n">
-        <v>212.6946035903898</v>
-      </c>
       <c r="D7" t="n">
-        <v>212.4243856737345</v>
+        <v>209.5294136496121</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45847.8125</v>
+        <v>45848.5625</v>
       </c>
       <c r="B8" t="n">
+        <v>212.0099945068359</v>
+      </c>
+      <c r="C8" t="n">
         <v>211.1100006103516</v>
       </c>
-      <c r="C8" t="n">
-        <v>207.0340039414726</v>
-      </c>
       <c r="D8" t="n">
-        <v>212.7776187528841</v>
+        <v>208.0585043743041</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45848.5625</v>
+        <v>45848.60416666666</v>
       </c>
       <c r="B9" t="n">
+        <v>212.9799957275391</v>
+      </c>
+      <c r="C9" t="n">
         <v>212.0099945068359</v>
       </c>
-      <c r="C9" t="n">
-        <v>211.2293018843458</v>
-      </c>
       <c r="D9" t="n">
-        <v>216.1614408011958</v>
+        <v>209.5979425958947</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45848.60416666666</v>
+        <v>45848.64583333334</v>
       </c>
       <c r="B10" t="n">
+        <v>212.0800018310547</v>
+      </c>
+      <c r="C10" t="n">
         <v>212.9799957275391</v>
       </c>
-      <c r="C10" t="n">
-        <v>210.9860288306324</v>
-      </c>
       <c r="D10" t="n">
-        <v>216.0533006294327</v>
+        <v>209.9980258609183</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45848.64583333334</v>
+        <v>45848.6875</v>
       </c>
       <c r="B11" t="n">
+        <v>212.6199951171875</v>
+      </c>
+      <c r="C11" t="n">
         <v>212.0800018310547</v>
       </c>
-      <c r="C11" t="n">
-        <v>213.4671792864045</v>
-      </c>
       <c r="D11" t="n">
-        <v>213.6341006946973</v>
+        <v>214.8890764744741</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45848.6875</v>
+        <v>45848.72916666666</v>
       </c>
       <c r="B12" t="n">
+        <v>212.6000061035156</v>
+      </c>
+      <c r="C12" t="n">
         <v>212.6199951171875</v>
       </c>
-      <c r="C12" t="n">
-        <v>211.315750870808</v>
-      </c>
       <c r="D12" t="n">
-        <v>213.3093383083494</v>
+        <v>207.067666099176</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45848.72916666666</v>
+        <v>45848.77083333334</v>
       </c>
       <c r="B13" t="n">
+        <v>212.5749969482422</v>
+      </c>
+      <c r="C13" t="n">
         <v>212.6000061035156</v>
       </c>
-      <c r="C13" t="n">
-        <v>215.2896586670746</v>
-      </c>
       <c r="D13" t="n">
-        <v>217.1173471254161</v>
+        <v>209.586717867964</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45848.77083333334</v>
+        <v>45848.8125</v>
       </c>
       <c r="B14" t="n">
+        <v>212.4199981689453</v>
+      </c>
+      <c r="C14" t="n">
         <v>212.5749969482422</v>
       </c>
-      <c r="C14" t="n">
-        <v>207.3169068619704</v>
-      </c>
       <c r="D14" t="n">
-        <v>209.5708731642876</v>
+        <v>214.3841571570057</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45848.8125</v>
+        <v>45849.5625</v>
       </c>
       <c r="B15" t="n">
+        <v>211.7899932861328</v>
+      </c>
+      <c r="C15" t="n">
         <v>212.4199981689453</v>
       </c>
-      <c r="C15" t="n">
-        <v>210.13923664136</v>
-      </c>
       <c r="D15" t="n">
-        <v>208.4092287155842</v>
+        <v>214.0784842464163</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45849.5625</v>
+        <v>45849.60416666666</v>
       </c>
       <c r="B16" t="n">
+        <v>210.8249969482422</v>
+      </c>
+      <c r="C16" t="n">
         <v>211.7899932861328</v>
       </c>
-      <c r="C16" t="n">
-        <v>212.3571252474565</v>
-      </c>
       <c r="D16" t="n">
-        <v>210.7652315962123</v>
+        <v>207.416602760971</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45849.60416666666</v>
+        <v>45849.64583333334</v>
       </c>
       <c r="B17" t="n">
+        <v>210.6349945068359</v>
+      </c>
+      <c r="C17" t="n">
         <v>210.8249969482422</v>
       </c>
-      <c r="C17" t="n">
-        <v>212.0275276204721</v>
-      </c>
       <c r="D17" t="n">
-        <v>216.0146832553101</v>
+        <v>208.2199641111351</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45849.64583333334</v>
+        <v>45849.6875</v>
       </c>
       <c r="B18" t="n">
+        <v>211.1649932861328</v>
+      </c>
+      <c r="C18" t="n">
         <v>210.6349945068359</v>
       </c>
-      <c r="C18" t="n">
-        <v>212.0294768517829</v>
-      </c>
       <c r="D18" t="n">
-        <v>218.6645550915982</v>
+        <v>216.6839633550513</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45849.6875</v>
+        <v>45849.72916666666</v>
       </c>
       <c r="B19" t="n">
+        <v>211.4049987792969</v>
+      </c>
+      <c r="C19" t="n">
         <v>211.1649932861328</v>
       </c>
-      <c r="C19" t="n">
-        <v>208.9499929470616</v>
-      </c>
       <c r="D19" t="n">
-        <v>213.0863152264002</v>
+        <v>211.8546269106953</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45849.72916666666</v>
+        <v>45849.77083333334</v>
       </c>
       <c r="B20" t="n">
+        <v>211.1600036621094</v>
+      </c>
+      <c r="C20" t="n">
         <v>211.4049987792969</v>
       </c>
-      <c r="C20" t="n">
-        <v>209.2596543709482</v>
-      </c>
       <c r="D20" t="n">
-        <v>214.1098338991944</v>
+        <v>213.880629082019</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45849.77083333334</v>
+        <v>45849.8125</v>
       </c>
       <c r="B21" t="n">
+        <v>211.0749969482422</v>
+      </c>
+      <c r="C21" t="n">
         <v>211.1600036621094</v>
       </c>
-      <c r="C21" t="n">
-        <v>210.9537604849728</v>
-      </c>
       <c r="D21" t="n">
-        <v>206.2399867466696</v>
+        <v>206.4115685202648</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45849.8125</v>
+        <v>45852.5625</v>
       </c>
       <c r="B22" t="n">
+        <v>208.0299987792969</v>
+      </c>
+      <c r="C22" t="n">
         <v>211.0749969482422</v>
       </c>
-      <c r="C22" t="n">
-        <v>216.4755414149191</v>
-      </c>
       <c r="D22" t="n">
-        <v>205.4980419969553</v>
+        <v>212.7758078496427</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45852.5625</v>
+        <v>45852.60416666666</v>
       </c>
       <c r="B23" t="n">
+        <v>208.7649993896484</v>
+      </c>
+      <c r="C23" t="n">
         <v>208.0299987792969</v>
       </c>
-      <c r="C23" t="n">
-        <v>214.2239087603494</v>
-      </c>
       <c r="D23" t="n">
-        <v>207.0419588456663</v>
+        <v>211.7921301119123</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45852.60416666666</v>
+        <v>45852.64583333334</v>
       </c>
       <c r="B24" t="n">
+        <v>208.8406982421875</v>
+      </c>
+      <c r="C24" t="n">
         <v>208.7649993896484</v>
       </c>
-      <c r="C24" t="n">
-        <v>203.7511580046325</v>
-      </c>
       <c r="D24" t="n">
-        <v>216.6618472041962</v>
+        <v>207.6747298772758</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45852.64583333334</v>
+        <v>45852.6875</v>
       </c>
       <c r="B25" t="n">
+        <v>209</v>
+      </c>
+      <c r="C25" t="n">
         <v>208.8406982421875</v>
       </c>
-      <c r="C25" t="n">
-        <v>207.997844348145</v>
-      </c>
       <c r="D25" t="n">
-        <v>210.6966718995407</v>
+        <v>211.6665997934498</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45852.6875</v>
+        <v>45852.72916666666</v>
       </c>
       <c r="B26" t="n">
         <v>209</v>
       </c>
       <c r="C26" t="n">
-        <v>211.755892941435</v>
+        <v>209</v>
       </c>
       <c r="D26" t="n">
-        <v>209.4239858347011</v>
+        <v>208.2140065425759</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45852.72916666666</v>
+        <v>45852.77083333334</v>
       </c>
       <c r="B27" t="n">
+        <v>209.1999053955078</v>
+      </c>
+      <c r="C27" t="n">
         <v>209</v>
       </c>
-      <c r="C27" t="n">
-        <v>209.0855543786186</v>
-      </c>
       <c r="D27" t="n">
-        <v>213.2246177477947</v>
+        <v>212.8942053003424</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45852.77083333334</v>
+        <v>45852.8125</v>
       </c>
       <c r="B28" t="n">
+        <v>208.5399932861328</v>
+      </c>
+      <c r="C28" t="n">
         <v>209.1999053955078</v>
       </c>
-      <c r="C28" t="n">
-        <v>205.4401652790321</v>
-      </c>
       <c r="D28" t="n">
-        <v>207.3739815812816</v>
+        <v>214.5460316979326</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45852.8125</v>
+        <v>45853.5625</v>
       </c>
       <c r="B29" t="n">
+        <v>210.1699981689453</v>
+      </c>
+      <c r="C29" t="n">
         <v>208.5399932861328</v>
       </c>
-      <c r="C29" t="n">
-        <v>209.8199252526369</v>
-      </c>
       <c r="D29" t="n">
-        <v>207.1361125076596</v>
+        <v>213.3241945868067</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45853.5625</v>
+        <v>45853.60416666666</v>
       </c>
       <c r="B30" t="n">
+        <v>211.4299926757812</v>
+      </c>
+      <c r="C30" t="n">
         <v>210.1699981689453</v>
       </c>
-      <c r="C30" t="n">
-        <v>211.5356189406893</v>
-      </c>
       <c r="D30" t="n">
-        <v>204.0569030826392</v>
+        <v>206.1443109000217</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45853.60416666666</v>
+        <v>45853.64583333334</v>
       </c>
       <c r="B31" t="n">
+        <v>210.6799926757812</v>
+      </c>
+      <c r="C31" t="n">
         <v>211.4299926757812</v>
       </c>
-      <c r="C31" t="n">
-        <v>209.209694483618</v>
-      </c>
       <c r="D31" t="n">
-        <v>210.0251484353505</v>
+        <v>212.4125054596048</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45853.64583333334</v>
+        <v>45853.6875</v>
       </c>
       <c r="B32" t="n">
+        <v>210.6726989746094</v>
+      </c>
+      <c r="C32" t="n">
         <v>210.6799926757812</v>
       </c>
-      <c r="C32" t="n">
-        <v>209.8029110039024</v>
-      </c>
       <c r="D32" t="n">
-        <v>213.5457763241716</v>
+        <v>211.4057365283323</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45853.6875</v>
+        <v>45853.72916666666</v>
       </c>
       <c r="B33" t="n">
+        <v>211.375</v>
+      </c>
+      <c r="C33" t="n">
         <v>210.6726989746094</v>
       </c>
-      <c r="C33" t="n">
-        <v>210.2023265714653</v>
-      </c>
       <c r="D33" t="n">
-        <v>212.4387874448975</v>
+        <v>216.4175418824649</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45853.72916666666</v>
+        <v>45853.77083333334</v>
       </c>
       <c r="B34" t="n">
+        <v>210.1799926757812</v>
+      </c>
+      <c r="C34" t="n">
         <v>211.375</v>
       </c>
-      <c r="C34" t="n">
-        <v>215.8412222408945</v>
-      </c>
       <c r="D34" t="n">
-        <v>210.3146203527614</v>
+        <v>208.5729180807568</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45853.77083333334</v>
+        <v>45853.8125</v>
       </c>
       <c r="B35" t="n">
+        <v>209.0099945068359</v>
+      </c>
+      <c r="C35" t="n">
         <v>210.1799926757812</v>
       </c>
-      <c r="C35" t="n">
-        <v>207.807060478153</v>
-      </c>
       <c r="D35" t="n">
-        <v>216.1023127594099</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>45853.8125</v>
-      </c>
-      <c r="B36" t="n">
-        <v>209.0099945068359</v>
-      </c>
-      <c r="C36" t="n">
-        <v>208.5205772793462</v>
-      </c>
-      <c r="D36" t="n">
-        <v>211.7789577138246</v>
+        <v>211.8234553491991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>